<commit_message>
averaged left & right
</commit_message>
<xml_diff>
--- a/fMRI-anovas/data/NMxPositiveAccuracy_anova3way.xlsx
+++ b/fMRI-anovas/data/NMxPositiveAccuracy_anova3way.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/neuromelanin/NMxAccuracy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/neuromelanin/fMRI-anovas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE267A84-5701-DD44-A6CB-1DD46DD0FAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FBC1EF-7AF8-694E-84DE-6720842CC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37660" yWindow="3400" windowWidth="25600" windowHeight="14760" xr2:uid="{79B66A3E-72FC-BE4A-89D9-CD830D2D4145}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14820" xr2:uid="{79B66A3E-72FC-BE4A-89D9-CD830D2D4145}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="51">
   <si>
     <t>Subject</t>
   </si>
@@ -173,6 +182,12 @@
   <si>
     <t>NM_full</t>
   </si>
+  <si>
+    <t>Ventral</t>
+  </si>
+  <si>
+    <t>Dorsal</t>
+  </si>
 </sst>
 </file>
 
@@ -207,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -331,11 +346,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -361,6 +389,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,15 +709,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31723B7A-45ED-944A-9BE0-99732653F64A}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -714,8 +748,14 @@
       <c r="J1" s="13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -746,8 +786,16 @@
       <c r="J2" s="2">
         <v>-5.9027999999999997E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <f>AVERAGE(G2,H2)</f>
+        <v>-9.6953000000000011E-2</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(I2,J2)</f>
+        <v>-6.6376999999999992E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -778,8 +826,16 @@
       <c r="J3" s="2">
         <v>-2.3734000000000002E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="0">AVERAGE(G3,H3)</f>
+        <v>-4.4757000000000005E-2</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L66" si="1">AVERAGE(I3,J3)</f>
+        <v>1.8258999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -810,8 +866,16 @@
       <c r="J4" s="2">
         <v>-3.6502E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>-8.9199000000000001E-2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>-1.5273E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -842,8 +906,16 @@
       <c r="J5" s="2">
         <v>0.10002</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>-2.5585499999999997E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>7.7536999999999995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -874,8 +946,16 @@
       <c r="J6" s="2">
         <v>3.9179999999999996E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-0.30197600000000002</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>4.5526000000000004E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -906,8 +986,16 @@
       <c r="J7" s="2">
         <v>-9.2687000000000005E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>-0.17773949999999999</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>-9.7758000000000012E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -938,8 +1026,16 @@
       <c r="J8" s="2">
         <v>3.5227000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>-4.2699500000000001E-2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>5.3605000000000007E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -970,8 +1066,16 @@
       <c r="J9" s="2">
         <v>4.4574000000000003E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>1.8943499999999999E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>6.595100000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1002,8 +1106,16 @@
       <c r="J10" s="2">
         <v>6.5639000000000003E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>-1.8413499999999999E-2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>3.7177500000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1034,8 +1146,16 @@
       <c r="J11" s="2">
         <v>-0.15962899999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>-3.0740999999999997E-2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>-0.23769400000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1066,8 +1186,16 @@
       <c r="J12" s="2">
         <v>-0.138872</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>-0.235064</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>-0.136906</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1098,8 +1226,16 @@
       <c r="J13" s="2">
         <v>-0.17643600000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>-0.27285700000000002</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>-0.22975400000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1130,8 +1266,16 @@
       <c r="J14" s="2">
         <v>5.0214000000000002E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>-8.2378000000000007E-2</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>1.2757500000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1162,8 +1306,16 @@
       <c r="J15" s="2">
         <v>6.3673999999999994E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>9.95085E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>6.3800499999999996E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1194,8 +1346,16 @@
       <c r="J16" s="2">
         <v>-5.1285999999999998E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>-4.1527000000000001E-2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>-7.9314999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1226,8 +1386,16 @@
       <c r="J17" s="2">
         <v>1.4598E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>-0.1514675</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>-3.9558999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1258,8 +1426,16 @@
       <c r="J18" s="2">
         <v>8.5816000000000003E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>6.8585000000000007E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>7.7403E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1290,8 +1466,16 @@
       <c r="J19" s="2">
         <v>2.6165999999999998E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>-5.9248000000000002E-2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>4.4795999999999996E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1322,8 +1506,16 @@
       <c r="J20" s="2">
         <v>-2.7833E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>1.0822E-2</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>-1.7061E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1354,8 +1546,16 @@
       <c r="J21" s="2">
         <v>3.0948E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>0.1214655</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>4.6637499999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1386,8 +1586,16 @@
       <c r="J22" s="2">
         <v>-7.0663000000000004E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>-0.163326</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>-0.132187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1418,8 +1626,16 @@
       <c r="J23" s="2">
         <v>-1.7505E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>-7.0611499999999994E-2</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>6.1749999999999999E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1450,8 +1666,16 @@
       <c r="J24" s="2">
         <v>-4.0952000000000002E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>-9.2540499999999998E-2</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>-0.1017605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1482,8 +1706,16 @@
       <c r="J25" s="2">
         <v>-7.4638999999999997E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>-0.17187150000000001</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>-0.1010665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1514,8 +1746,16 @@
       <c r="J26" s="2">
         <v>8.3649000000000001E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>-1.6561000000000003E-2</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>5.1922000000000003E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1546,8 +1786,16 @@
       <c r="J27" s="2">
         <v>-0.13892099999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>-0.162936</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>-0.14506449999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1578,8 +1826,16 @@
       <c r="J28" s="2">
         <v>-3.3774999999999999E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>-0.15967600000000001</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>4.6128500000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1610,8 +1866,16 @@
       <c r="J29" s="2">
         <v>-9.2040999999999998E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>-4.1850999999999999E-2</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>-0.12528</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1642,8 +1906,16 @@
       <c r="J30" s="2">
         <v>-6.9511000000000003E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>-0.19819799999999999</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>-7.5264500000000012E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1674,8 +1946,16 @@
       <c r="J31" s="2">
         <v>-2.3716999999999998E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>-0.19357799999999997</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>-1.7041999999999998E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -1706,8 +1986,16 @@
       <c r="J32" s="2">
         <v>-5.1005000000000002E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>2.3279000000000001E-2</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>-2.7189500000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1738,8 +2026,16 @@
       <c r="J33" s="2">
         <v>-0.10000299999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>-0.140926</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>-0.13221749999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -1770,8 +2066,16 @@
       <c r="J34" s="2">
         <v>0.12664800000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>9.9430000000000004E-3</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>0.12137000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -1802,8 +2106,16 @@
       <c r="J35" s="2">
         <v>-8.1860000000000002E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>-0.16462749999999998</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>-0.139573</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -1834,8 +2146,16 @@
       <c r="J36" s="2">
         <v>6.8223000000000006E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>5.8689999999999999E-2</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>6.0819499999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
@@ -1866,8 +2186,16 @@
       <c r="J37" s="2">
         <v>6.9194000000000006E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>-0.1300385</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>4.3566000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1898,8 +2226,16 @@
       <c r="J38" s="2">
         <v>9.2760999999999996E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>0.20445249999999998</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>0.14322399999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -1930,8 +2266,16 @@
       <c r="J39" s="2">
         <v>-6.4127000000000003E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>-0.1692205</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>-4.1827500000000004E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1962,8 +2306,16 @@
       <c r="J40" s="2">
         <v>9.3731999999999996E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>0.2122675</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>8.5449499999999998E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
@@ -1994,8 +2346,16 @@
       <c r="J41" s="2">
         <v>-1.4874999999999999E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>-0.14957500000000001</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="1"/>
+        <v>2.2869500000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -2026,8 +2386,16 @@
       <c r="J42" s="2">
         <v>7.8172000000000005E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>2.5348500000000003E-2</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>3.6233500000000002E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -2058,8 +2426,16 @@
       <c r="J43" s="2">
         <v>0.10079100000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>2.6543500000000001E-2</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="1"/>
+        <v>5.2115500000000002E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -2090,8 +2466,16 @@
       <c r="J44" s="2">
         <v>7.3447999999999999E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>3.6229499999999998E-2</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="1"/>
+        <v>5.1860999999999997E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -2122,8 +2506,16 @@
       <c r="J45" s="2">
         <v>3.0689999999999999E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>-7.6849499999999987E-2</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>2.0375499999999998E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>11</v>
       </c>
@@ -2154,8 +2546,16 @@
       <c r="J46" s="2">
         <v>-2.0787E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>0.13872950000000001</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>-3.7075999999999998E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>12</v>
       </c>
@@ -2186,8 +2586,16 @@
       <c r="J47" s="2">
         <v>-2.4535000000000001E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>-9.6784000000000009E-2</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>-5.0932499999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>13</v>
       </c>
@@ -2218,8 +2626,16 @@
       <c r="J48" s="2">
         <v>0.11176899999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <f t="shared" si="0"/>
+        <v>0.16839500000000002</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="1"/>
+        <v>0.10262099999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
@@ -2250,8 +2666,16 @@
       <c r="J49" s="2">
         <v>5.8465000000000003E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>0.1037415</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="1"/>
+        <v>3.4941E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
@@ -2282,8 +2706,16 @@
       <c r="J50" s="2">
         <v>0.23819199999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <f t="shared" si="0"/>
+        <v>8.7649000000000005E-2</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="1"/>
+        <v>0.23391849999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>16</v>
       </c>
@@ -2314,8 +2746,16 @@
       <c r="J51" s="2">
         <v>1.9552E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <f t="shared" si="0"/>
+        <v>6.2715999999999994E-2</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="1"/>
+        <v>-2.4447000000000003E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -2346,8 +2786,16 @@
       <c r="J52" s="2">
         <v>6.6969999999999998E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <f t="shared" si="0"/>
+        <v>-6.5981499999999998E-2</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="1"/>
+        <v>-1.7991500000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>18</v>
       </c>
@@ -2378,8 +2826,16 @@
       <c r="J53" s="2">
         <v>4.1669999999999997E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <f t="shared" si="0"/>
+        <v>-2.5538999999999999E-2</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="1"/>
+        <v>-1.711E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>19</v>
       </c>
@@ -2410,8 +2866,16 @@
       <c r="J54" s="2">
         <v>8.0058000000000004E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <f t="shared" si="0"/>
+        <v>2.03115E-2</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="1"/>
+        <v>6.5834000000000004E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>20</v>
       </c>
@@ -2442,8 +2906,16 @@
       <c r="J55" s="2">
         <v>-2.7099999999999997E-4</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>2.0958499999999998E-2</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="1"/>
+        <v>2.7310999999999998E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>21</v>
       </c>
@@ -2474,8 +2946,16 @@
       <c r="J56" s="2">
         <v>6.0911E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <f t="shared" si="0"/>
+        <v>4.812799999999999E-2</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="1"/>
+        <v>6.3338000000000005E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>22</v>
       </c>
@@ -2506,8 +2986,16 @@
       <c r="J57" s="2">
         <v>-7.2345000000000007E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <f t="shared" si="0"/>
+        <v>-3.5323E-2</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="1"/>
+        <v>-7.2483000000000006E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>23</v>
       </c>
@@ -2538,8 +3026,16 @@
       <c r="J58" s="2">
         <v>4.8473000000000002E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <f t="shared" si="0"/>
+        <v>4.5471999999999999E-2</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="1"/>
+        <v>6.9178000000000003E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
@@ -2570,8 +3066,16 @@
       <c r="J59" s="2">
         <v>1.6598999999999999E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <f t="shared" si="0"/>
+        <v>2.0188000000000001E-2</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="1"/>
+        <v>-1.33305E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>25</v>
       </c>
@@ -2602,8 +3106,16 @@
       <c r="J60" s="2">
         <v>4.0099999999999997E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <f t="shared" si="0"/>
+        <v>-2.2508999999999994E-2</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="1"/>
+        <v>1.7735499999999998E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>26</v>
       </c>
@@ -2634,8 +3146,16 @@
       <c r="J61" s="2">
         <v>0.19259299999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <f t="shared" si="0"/>
+        <v>0.23388150000000002</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="1"/>
+        <v>0.14033000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>27</v>
       </c>
@@ -2666,8 +3186,16 @@
       <c r="J62" s="2">
         <v>-6.5240999999999993E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <f t="shared" si="0"/>
+        <v>-2.8428500000000002E-2</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="1"/>
+        <v>-6.3338999999999993E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>28</v>
       </c>
@@ -2698,8 +3226,16 @@
       <c r="J63" s="2">
         <v>-1.9386E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <f t="shared" si="0"/>
+        <v>-3.1807500000000002E-2</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="1"/>
+        <v>4.6154999999999998E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>29</v>
       </c>
@@ -2730,8 +3266,16 @@
       <c r="J64" s="2">
         <v>8.5773000000000002E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <f t="shared" si="0"/>
+        <v>0.1047535</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="1"/>
+        <v>5.3642500000000003E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>30</v>
       </c>
@@ -2762,8 +3306,16 @@
       <c r="J65" s="2">
         <v>6.8507999999999999E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <f t="shared" si="0"/>
+        <v>2.034E-2</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="1"/>
+        <v>4.8063000000000002E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>31</v>
       </c>
@@ -2794,8 +3346,16 @@
       <c r="J66" s="2">
         <v>4.7199999999999998E-4</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <f t="shared" si="0"/>
+        <v>-9.7470000000000005E-3</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="1"/>
+        <v>2.8475000000000002E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>32</v>
       </c>
@@ -2826,8 +3386,16 @@
       <c r="J67" s="2">
         <v>7.8109999999999999E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <f t="shared" ref="K67:K130" si="2">AVERAGE(G67,H67)</f>
+        <v>0.12726299999999999</v>
+      </c>
+      <c r="L67">
+        <f t="shared" ref="L67:L130" si="3">AVERAGE(I67,J67)</f>
+        <v>6.7236500000000005E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
@@ -2858,8 +3426,16 @@
       <c r="J68" s="2">
         <v>3.7670000000000002E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <f t="shared" si="2"/>
+        <v>0.25682749999999999</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="3"/>
+        <v>-1.8767499999999996E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>34</v>
       </c>
@@ -2890,8 +3466,16 @@
       <c r="J69" s="2">
         <v>6.2628000000000003E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <f t="shared" si="2"/>
+        <v>-6.6050499999999998E-2</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="3"/>
+        <v>1.1983000000000001E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>35</v>
       </c>
@@ -2922,8 +3506,16 @@
       <c r="J70" s="2">
         <v>-5.527E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <f t="shared" si="2"/>
+        <v>-0.23227700000000001</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="3"/>
+        <v>-0.110206</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>36</v>
       </c>
@@ -2954,8 +3546,16 @@
       <c r="J71" s="2">
         <v>0.190882</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71">
+        <f t="shared" si="2"/>
+        <v>0.16444400000000001</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="3"/>
+        <v>0.161913</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>2</v>
       </c>
@@ -2986,8 +3586,16 @@
       <c r="J72" s="2">
         <v>5.0793999999999999E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <f t="shared" si="2"/>
+        <v>2.6477000000000001E-2</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="3"/>
+        <v>7.9358499999999998E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
@@ -3018,8 +3626,16 @@
       <c r="J73" s="2">
         <v>1.8766999999999999E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <f t="shared" si="2"/>
+        <v>6.3779499999999989E-2</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="3"/>
+        <v>-3.3458500000000002E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>4</v>
       </c>
@@ -3050,8 +3666,16 @@
       <c r="J74" s="2">
         <v>-6.7714999999999997E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <f t="shared" si="2"/>
+        <v>-0.1249025</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="3"/>
+        <v>-9.7397499999999998E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
@@ -3082,8 +3706,16 @@
       <c r="J75" s="2">
         <v>8.6390000000000008E-3</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K75">
+        <f t="shared" si="2"/>
+        <v>-8.3361999999999992E-2</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="3"/>
+        <v>-2.4499E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -3114,8 +3746,16 @@
       <c r="J76" s="2">
         <v>0.154333</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K76">
+        <f t="shared" si="2"/>
+        <v>0.1046605</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="3"/>
+        <v>0.17442849999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -3146,8 +3786,16 @@
       <c r="J77" s="2">
         <v>-6.8348000000000006E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K77">
+        <f t="shared" si="2"/>
+        <v>-4.8764000000000002E-2</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="3"/>
+        <v>-6.9221500000000005E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>8</v>
       </c>
@@ -3178,8 +3826,16 @@
       <c r="J78" s="2">
         <v>-7.9360000000000003E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78">
+        <f t="shared" si="2"/>
+        <v>1.2653500000000002E-2</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="3"/>
+        <v>-5.0287499999999999E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
@@ -3210,8 +3866,16 @@
       <c r="J79" s="2">
         <v>-4.823E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79">
+        <f t="shared" si="2"/>
+        <v>-7.6527499999999998E-2</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="3"/>
+        <v>-1.9602000000000001E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>10</v>
       </c>
@@ -3242,8 +3906,16 @@
       <c r="J80" s="2">
         <v>-7.5482999999999995E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80">
+        <f t="shared" si="2"/>
+        <v>-0.1474705</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="3"/>
+        <v>-5.4846499999999992E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
@@ -3274,8 +3946,16 @@
       <c r="J81" s="2">
         <v>-4.3059E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81">
+        <f t="shared" si="2"/>
+        <v>-1.5414499999999998E-2</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="3"/>
+        <v>-2.9617499999999998E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>12</v>
       </c>
@@ -3306,8 +3986,16 @@
       <c r="J82" s="2">
         <v>4.6105E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K82">
+        <f t="shared" si="2"/>
+        <v>0.17693199999999998</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="3"/>
+        <v>5.4579500000000003E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>13</v>
       </c>
@@ -3338,8 +4026,16 @@
       <c r="J83" s="2">
         <v>-0.25545400000000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83">
+        <f t="shared" si="2"/>
+        <v>-0.18378549999999999</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="3"/>
+        <v>-0.2933055</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>14</v>
       </c>
@@ -3370,8 +4066,16 @@
       <c r="J84" s="2">
         <v>4.6669000000000002E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K84">
+        <f t="shared" si="2"/>
+        <v>4.2217499999999998E-2</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="3"/>
+        <v>3.2286500000000003E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>15</v>
       </c>
@@ -3402,8 +4106,16 @@
       <c r="J85" s="2">
         <v>8.5344000000000003E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85">
+        <f t="shared" si="2"/>
+        <v>-4.1463E-2</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="3"/>
+        <v>5.8516499999999999E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>16</v>
       </c>
@@ -3434,8 +4146,16 @@
       <c r="J86" s="2">
         <v>4.2819000000000003E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86">
+        <f t="shared" si="2"/>
+        <v>6.7418500000000006E-2</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="3"/>
+        <v>6.7324499999999995E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>17</v>
       </c>
@@ -3466,8 +4186,16 @@
       <c r="J87" s="2">
         <v>-6.9585999999999995E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87">
+        <f t="shared" si="2"/>
+        <v>-0.17781949999999999</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="3"/>
+        <v>-6.1627000000000001E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>18</v>
       </c>
@@ -3498,8 +4226,16 @@
       <c r="J88" s="2">
         <v>3.6924999999999999E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88">
+        <f t="shared" si="2"/>
+        <v>2.6152999999999999E-2</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="3"/>
+        <v>3.4648499999999999E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>19</v>
       </c>
@@ -3530,8 +4266,16 @@
       <c r="J89" s="2">
         <v>0.15524299999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89">
+        <f t="shared" si="2"/>
+        <v>0.2115735</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="3"/>
+        <v>0.126747</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>20</v>
       </c>
@@ -3562,8 +4306,16 @@
       <c r="J90" s="2">
         <v>-0.17955499999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90">
+        <f t="shared" si="2"/>
+        <v>-0.13117000000000001</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="3"/>
+        <v>-0.1866855</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>21</v>
       </c>
@@ -3594,8 +4346,16 @@
       <c r="J91" s="2">
         <v>-8.1141000000000005E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91">
+        <f t="shared" si="2"/>
+        <v>-0.11526549999999999</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="3"/>
+        <v>-5.9789500000000002E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>22</v>
       </c>
@@ -3626,8 +4386,16 @@
       <c r="J92" s="2">
         <v>-0.13891500000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92">
+        <f t="shared" si="2"/>
+        <v>-0.1274055</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="3"/>
+        <v>-0.167738</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>23</v>
       </c>
@@ -3658,8 +4426,16 @@
       <c r="J93" s="2">
         <v>-1.0194999999999999E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93">
+        <f t="shared" si="2"/>
+        <v>5.8583499999999997E-2</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="3"/>
+        <v>2.1701999999999999E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>24</v>
       </c>
@@ -3690,8 +4466,16 @@
       <c r="J94" s="2">
         <v>-0.180978</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94">
+        <f t="shared" si="2"/>
+        <v>-8.1425999999999998E-2</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="3"/>
+        <v>-0.25183899999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>25</v>
       </c>
@@ -3722,8 +4506,16 @@
       <c r="J95" s="2">
         <v>3.6181999999999999E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K95">
+        <f t="shared" si="2"/>
+        <v>8.8067000000000006E-2</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="3"/>
+        <v>2.4787500000000001E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>26</v>
       </c>
@@ -3754,8 +4546,16 @@
       <c r="J96" s="2">
         <v>3.1959000000000001E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96">
+        <f t="shared" si="2"/>
+        <v>2.2399999999999989E-3</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="3"/>
+        <v>4.0889999999999996E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>27</v>
       </c>
@@ -3786,8 +4586,16 @@
       <c r="J97" s="2">
         <v>2.2284999999999999E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97">
+        <f t="shared" si="2"/>
+        <v>-3.0700999999999999E-2</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="3"/>
+        <v>2.9114999999999999E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>28</v>
       </c>
@@ -3818,8 +4626,16 @@
       <c r="J98" s="2">
         <v>0.13467999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98">
+        <f t="shared" si="2"/>
+        <v>-0.16554950000000002</v>
+      </c>
+      <c r="L98">
+        <f t="shared" si="3"/>
+        <v>7.5396999999999992E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>29</v>
       </c>
@@ -3850,8 +4666,16 @@
       <c r="J99" s="2">
         <v>-6.1520999999999999E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99">
+        <f t="shared" si="2"/>
+        <v>3.2922E-2</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="3"/>
+        <v>-0.11129849999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>30</v>
       </c>
@@ -3882,8 +4706,16 @@
       <c r="J100" s="2">
         <v>0.13848099999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100">
+        <f t="shared" si="2"/>
+        <v>0.19856750000000001</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="3"/>
+        <v>0.12632650000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>31</v>
       </c>
@@ -3914,8 +4746,16 @@
       <c r="J101" s="2">
         <v>-0.15457199999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K101">
+        <f t="shared" si="2"/>
+        <v>-0.18417250000000002</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="3"/>
+        <v>-0.17441099999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>32</v>
       </c>
@@ -3946,8 +4786,16 @@
       <c r="J102" s="2">
         <v>-1.2631E-2</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K102">
+        <f t="shared" si="2"/>
+        <v>7.7974000000000002E-2</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="3"/>
+        <v>3.9590000000000007E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>33</v>
       </c>
@@ -3978,8 +4826,16 @@
       <c r="J103" s="2">
         <v>0.13563500000000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K103">
+        <f t="shared" si="2"/>
+        <v>0.249917</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="3"/>
+        <v>0.12787750000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>34</v>
       </c>
@@ -4010,8 +4866,16 @@
       <c r="J104" s="2">
         <v>-0.161796</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K104">
+        <f t="shared" si="2"/>
+        <v>-0.21374500000000002</v>
+      </c>
+      <c r="L104">
+        <f t="shared" si="3"/>
+        <v>-0.11158849999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>35</v>
       </c>
@@ -4042,8 +4906,16 @@
       <c r="J105" s="2">
         <v>7.5648000000000007E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K105">
+        <f t="shared" si="2"/>
+        <v>2.1119999999999993E-3</v>
+      </c>
+      <c r="L105">
+        <f t="shared" si="3"/>
+        <v>4.7274000000000004E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>36</v>
       </c>
@@ -4074,8 +4946,16 @@
       <c r="J106" s="2">
         <v>2.5399999999999999E-4</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K106">
+        <f t="shared" si="2"/>
+        <v>-4.3700000000000003E-2</v>
+      </c>
+      <c r="L106">
+        <f t="shared" si="3"/>
+        <v>1.7628499999999998E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>2</v>
       </c>
@@ -4106,8 +4986,16 @@
       <c r="J107" s="2">
         <v>0.103228</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K107">
+        <f t="shared" si="2"/>
+        <v>-2.8499E-2</v>
+      </c>
+      <c r="L107">
+        <f t="shared" si="3"/>
+        <v>9.0135999999999994E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
@@ -4138,8 +5026,16 @@
       <c r="J108" s="2">
         <v>0.105311</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K108">
+        <f t="shared" si="2"/>
+        <v>0.10961900000000001</v>
+      </c>
+      <c r="L108">
+        <f t="shared" si="3"/>
+        <v>7.9495999999999997E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>4</v>
       </c>
@@ -4170,8 +5066,16 @@
       <c r="J109" s="2">
         <v>0.148752</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K109">
+        <f t="shared" si="2"/>
+        <v>0.13337350000000001</v>
+      </c>
+      <c r="L109">
+        <f t="shared" si="3"/>
+        <v>0.12923599999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -4202,8 +5106,16 @@
       <c r="J110" s="2">
         <v>7.0703000000000002E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K110">
+        <f t="shared" si="2"/>
+        <v>0.1814935</v>
+      </c>
+      <c r="L110">
+        <f t="shared" si="3"/>
+        <v>8.39255E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>6</v>
       </c>
@@ -4234,8 +5146,16 @@
       <c r="J111" s="2">
         <v>0.17183999999999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K111">
+        <f t="shared" si="2"/>
+        <v>0.15199850000000001</v>
+      </c>
+      <c r="L111">
+        <f t="shared" si="3"/>
+        <v>0.19106049999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>7</v>
       </c>
@@ -4266,8 +5186,16 @@
       <c r="J112" s="2">
         <v>-2.4538000000000001E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K112">
+        <f t="shared" si="2"/>
+        <v>-4.3002499999999999E-2</v>
+      </c>
+      <c r="L112">
+        <f t="shared" si="3"/>
+        <v>-1.8894000000000001E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>8</v>
       </c>
@@ -4298,8 +5226,16 @@
       <c r="J113" s="2">
         <v>0.132909</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K113">
+        <f t="shared" si="2"/>
+        <v>0.1353705</v>
+      </c>
+      <c r="L113">
+        <f t="shared" si="3"/>
+        <v>0.1074295</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>9</v>
       </c>
@@ -4330,8 +5266,16 @@
       <c r="J114" s="2">
         <v>5.2283999999999997E-2</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K114">
+        <f t="shared" si="2"/>
+        <v>5.4734000000000005E-2</v>
+      </c>
+      <c r="L114">
+        <f t="shared" si="3"/>
+        <v>4.6152499999999999E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>10</v>
       </c>
@@ -4362,8 +5306,16 @@
       <c r="J115" s="2">
         <v>-5.8012000000000001E-2</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K115">
+        <f t="shared" si="2"/>
+        <v>-7.6815500000000009E-2</v>
+      </c>
+      <c r="L115">
+        <f t="shared" si="3"/>
+        <v>-7.0218000000000003E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>11</v>
       </c>
@@ -4394,8 +5346,16 @@
       <c r="J116" s="2">
         <v>9.4061000000000006E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K116">
+        <f t="shared" si="2"/>
+        <v>3.7094500000000002E-2</v>
+      </c>
+      <c r="L116">
+        <f t="shared" si="3"/>
+        <v>0.105819</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
@@ -4426,8 +5386,16 @@
       <c r="J117" s="2">
         <v>0.137603</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K117">
+        <f t="shared" si="2"/>
+        <v>8.2685499999999995E-2</v>
+      </c>
+      <c r="L117">
+        <f t="shared" si="3"/>
+        <v>0.17643049999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>13</v>
       </c>
@@ -4458,8 +5426,16 @@
       <c r="J118" s="2">
         <v>8.3829999999999998E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K118">
+        <f t="shared" si="2"/>
+        <v>9.5372499999999999E-2</v>
+      </c>
+      <c r="L118">
+        <f t="shared" si="3"/>
+        <v>-5.3498499999999997E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>14</v>
       </c>
@@ -4490,8 +5466,16 @@
       <c r="J119" s="2">
         <v>8.4153000000000006E-2</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K119">
+        <f t="shared" si="2"/>
+        <v>0.14825250000000001</v>
+      </c>
+      <c r="L119">
+        <f t="shared" si="3"/>
+        <v>6.0884000000000008E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>15</v>
       </c>
@@ -4522,8 +5506,16 @@
       <c r="J120" s="2">
         <v>0.13961200000000001</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K120">
+        <f t="shared" si="2"/>
+        <v>-1.0112000000000001E-2</v>
+      </c>
+      <c r="L120">
+        <f t="shared" si="3"/>
+        <v>9.77885E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>16</v>
       </c>
@@ -4554,8 +5546,16 @@
       <c r="J121" s="2">
         <v>7.9843999999999998E-2</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K121">
+        <f t="shared" si="2"/>
+        <v>0.17668149999999999</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="3"/>
+        <v>7.2880500000000001E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>17</v>
       </c>
@@ -4586,8 +5586,16 @@
       <c r="J122" s="2">
         <v>-0.186363</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K122">
+        <f t="shared" si="2"/>
+        <v>-0.104079</v>
+      </c>
+      <c r="L122">
+        <f t="shared" si="3"/>
+        <v>-0.16324549999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>18</v>
       </c>
@@ -4618,8 +5626,16 @@
       <c r="J123" s="2">
         <v>0.131714</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K123">
+        <f t="shared" si="2"/>
+        <v>0.21639549999999999</v>
+      </c>
+      <c r="L123">
+        <f t="shared" si="3"/>
+        <v>0.136488</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>19</v>
       </c>
@@ -4650,8 +5666,16 @@
       <c r="J124" s="2">
         <v>-3.0850000000000001E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K124">
+        <f t="shared" si="2"/>
+        <v>0.1026715</v>
+      </c>
+      <c r="L124">
+        <f t="shared" si="3"/>
+        <v>2.2243500000000003E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>20</v>
       </c>
@@ -4682,8 +5706,16 @@
       <c r="J125" s="2">
         <v>-0.243644</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K125">
+        <f t="shared" si="2"/>
+        <v>-0.1577345</v>
+      </c>
+      <c r="L125">
+        <f t="shared" si="3"/>
+        <v>-0.2337545</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>21</v>
       </c>
@@ -4714,8 +5746,16 @@
       <c r="J126" s="2">
         <v>0.148115</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K126">
+        <f t="shared" si="2"/>
+        <v>0.16419149999999999</v>
+      </c>
+      <c r="L126">
+        <f t="shared" si="3"/>
+        <v>0.1382755</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>22</v>
       </c>
@@ -4746,8 +5786,16 @@
       <c r="J127" s="2">
         <v>-0.101881</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K127">
+        <f t="shared" si="2"/>
+        <v>-0.16868549999999999</v>
+      </c>
+      <c r="L127">
+        <f t="shared" si="3"/>
+        <v>-0.13276350000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>23</v>
       </c>
@@ -4778,8 +5826,16 @@
       <c r="J128" s="2">
         <v>-6.5180000000000004E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K128">
+        <f t="shared" si="2"/>
+        <v>0.108737</v>
+      </c>
+      <c r="L128">
+        <f t="shared" si="3"/>
+        <v>3.3605500000000003E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>24</v>
       </c>
@@ -4810,8 +5866,16 @@
       <c r="J129" s="2">
         <v>2.1330999999999999E-2</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K129">
+        <f t="shared" si="2"/>
+        <v>4.2142499999999999E-2</v>
+      </c>
+      <c r="L129">
+        <f t="shared" si="3"/>
+        <v>-4.95115E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>25</v>
       </c>
@@ -4842,8 +5906,16 @@
       <c r="J130" s="2">
         <v>9.5702999999999996E-2</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K130">
+        <f t="shared" si="2"/>
+        <v>7.3749499999999996E-2</v>
+      </c>
+      <c r="L130">
+        <f t="shared" si="3"/>
+        <v>0.123367</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>26</v>
       </c>
@@ -4874,8 +5946,16 @@
       <c r="J131" s="2">
         <v>0.161245</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K131">
+        <f t="shared" ref="K131:K141" si="4">AVERAGE(G131,H131)</f>
+        <v>9.0142E-2</v>
+      </c>
+      <c r="L131">
+        <f t="shared" ref="L131:L141" si="5">AVERAGE(I131,J131)</f>
+        <v>0.14987149999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>27</v>
       </c>
@@ -4906,8 +5986,16 @@
       <c r="J132" s="2">
         <v>-0.123275</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K132">
+        <f t="shared" si="4"/>
+        <v>-0.12122250000000001</v>
+      </c>
+      <c r="L132">
+        <f t="shared" si="5"/>
+        <v>-9.6172999999999995E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>28</v>
       </c>
@@ -4938,8 +6026,16 @@
       <c r="J133" s="2">
         <v>0.19463</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K133">
+        <f t="shared" si="4"/>
+        <v>6.5114499999999992E-2</v>
+      </c>
+      <c r="L133">
+        <f t="shared" si="5"/>
+        <v>0.15516199999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>29</v>
       </c>
@@ -4970,8 +6066,16 @@
       <c r="J134" s="2">
         <v>-4.7421999999999999E-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K134">
+        <f t="shared" si="4"/>
+        <v>0.14030500000000001</v>
+      </c>
+      <c r="L134">
+        <f t="shared" si="5"/>
+        <v>-6.7985000000000004E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>30</v>
       </c>
@@ -5002,8 +6106,16 @@
       <c r="J135" s="2">
         <v>0.122512</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K135">
+        <f t="shared" si="4"/>
+        <v>0.10000450000000001</v>
+      </c>
+      <c r="L135">
+        <f t="shared" si="5"/>
+        <v>0.12936</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>31</v>
       </c>
@@ -5034,8 +6146,16 @@
       <c r="J136" s="2">
         <v>0.156164</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K136">
+        <f t="shared" si="4"/>
+        <v>0.2201245</v>
+      </c>
+      <c r="L136">
+        <f t="shared" si="5"/>
+        <v>0.1681745</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>32</v>
       </c>
@@ -5066,8 +6186,16 @@
       <c r="J137" s="2">
         <v>-4.5734999999999998E-2</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K137">
+        <f t="shared" si="4"/>
+        <v>1.07595E-2</v>
+      </c>
+      <c r="L137">
+        <f t="shared" si="5"/>
+        <v>-1.8960499999999998E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>33</v>
       </c>
@@ -5098,8 +6226,16 @@
       <c r="J138" s="2">
         <v>0.18754899999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K138">
+        <f t="shared" si="4"/>
+        <v>-5.6598999999999997E-2</v>
+      </c>
+      <c r="L138">
+        <f t="shared" si="5"/>
+        <v>0.17669699999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>34</v>
       </c>
@@ -5130,8 +6266,16 @@
       <c r="J139" s="2">
         <v>-9.8267999999999994E-2</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K139">
+        <f t="shared" si="4"/>
+        <v>-7.7405499999999988E-2</v>
+      </c>
+      <c r="L139">
+        <f t="shared" si="5"/>
+        <v>-7.613049999999999E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>35</v>
       </c>
@@ -5162,8 +6306,16 @@
       <c r="J140" s="2">
         <v>2.2464000000000001E-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K140">
+        <f t="shared" si="4"/>
+        <v>-4.8635500000000005E-2</v>
+      </c>
+      <c r="L140">
+        <f t="shared" si="5"/>
+        <v>-2.8743999999999999E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>36</v>
       </c>
@@ -5193,6 +6345,14 @@
       </c>
       <c r="J141" s="5">
         <v>-3.39E-4</v>
+      </c>
+      <c r="K141">
+        <f t="shared" si="4"/>
+        <v>-8.0625000000000002E-3</v>
+      </c>
+      <c r="L141">
+        <f t="shared" si="5"/>
+        <v>1.48185E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>